<commit_message>
fixed start finish TE height calculation. Using 60kt finish speed, 91kt start speeds, and TE correction factor of 0.8.
Changed  Rule2_time_behind_rank1 time calculation to be based on rank1's total_thermal_time.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -769,7 +769,7 @@
         <v>9.51</v>
       </c>
       <c r="V2" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="W2" t="n">
         <v>121</v>
@@ -781,7 +781,7 @@
         <v>8.17</v>
       </c>
       <c r="Z2" t="n">
-        <v>321</v>
+        <v>413</v>
       </c>
       <c r="AA2" t="n">
         <v>184.29</v>
@@ -930,7 +930,7 @@
         <v>9.07</v>
       </c>
       <c r="V3" t="n">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="W3" t="n">
         <v>80</v>
@@ -942,7 +942,7 @@
         <v>8.710000000000001</v>
       </c>
       <c r="Z3" t="n">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="AA3" t="n">
         <v>182.94</v>
@@ -995,7 +995,7 @@
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>'00:14</t>
+          <t>'-00:11</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
@@ -1015,12 +1015,12 @@
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>'00:03</t>
+          <t>'00:04</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
         <is>
-          <t>'-00:02</t>
+          <t>'-00:10</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
         <v>8.779999999999999</v>
       </c>
       <c r="V4" t="n">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="W4" t="n">
         <v>135</v>
@@ -1103,7 +1103,7 @@
         <v>7.49</v>
       </c>
       <c r="Z4" t="n">
-        <v>429</v>
+        <v>606</v>
       </c>
       <c r="AA4" t="n">
         <v>179.79</v>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>'-2:37</t>
+          <t>'-01:22</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
@@ -1176,12 +1176,12 @@
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>'00:04</t>
+          <t>'00:03</t>
         </is>
       </c>
       <c r="AQ4" t="inlineStr">
         <is>
-          <t>'00:03</t>
+          <t>'00:09</t>
         </is>
       </c>
     </row>
@@ -1252,7 +1252,7 @@
         <v>9.15</v>
       </c>
       <c r="V5" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="W5" t="n">
         <v>130</v>
@@ -1264,7 +1264,7 @@
         <v>7.77</v>
       </c>
       <c r="Z5" t="n">
-        <v>376</v>
+        <v>519</v>
       </c>
       <c r="AA5" t="n">
         <v>179.59</v>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>'00:06</t>
+          <t>'-00:38</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="AQ5" t="inlineStr">
         <is>
-          <t>'00:02</t>
+          <t>'00:07</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
         <v>9.539999999999999</v>
       </c>
       <c r="V6" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W6" t="n">
         <v>91</v>
@@ -1425,7 +1425,7 @@
         <v>8.859999999999999</v>
       </c>
       <c r="Z6" t="n">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="AA6" t="n">
         <v>178.66</v>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>'00:51</t>
+          <t>'-00:08</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="AQ6" t="inlineStr">
         <is>
-          <t>'-00:07</t>
+          <t>'-00:15</t>
         </is>
       </c>
     </row>
@@ -1574,7 +1574,7 @@
         <v>8.31</v>
       </c>
       <c r="V7" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="W7" t="n">
         <v>152</v>
@@ -1586,7 +1586,7 @@
         <v>7.13</v>
       </c>
       <c r="Z7" t="n">
-        <v>374</v>
+        <v>697</v>
       </c>
       <c r="AA7" t="n">
         <v>178</v>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>'-1:43</t>
+          <t>'-00:38</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
@@ -1659,12 +1659,12 @@
       </c>
       <c r="AP7" t="inlineStr">
         <is>
-          <t>'00:08</t>
+          <t>'00:07</t>
         </is>
       </c>
       <c r="AQ7" t="inlineStr">
         <is>
-          <t>'00:02</t>
+          <t>'00:24</t>
         </is>
       </c>
     </row>
@@ -1735,7 +1735,7 @@
         <v>8.35</v>
       </c>
       <c r="V8" t="n">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="W8" t="n">
         <v>115</v>
@@ -1747,7 +1747,7 @@
         <v>7.95</v>
       </c>
       <c r="Z8" t="n">
-        <v>428</v>
+        <v>494</v>
       </c>
       <c r="AA8" t="n">
         <v>177.86</v>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>'00:02</t>
+          <t>'-00:34</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
@@ -1820,12 +1820,12 @@
       </c>
       <c r="AP8" t="inlineStr">
         <is>
-          <t>'00:08</t>
+          <t>'00:07</t>
         </is>
       </c>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>'00:08</t>
+          <t>'00:05</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
         <v>8.92</v>
       </c>
       <c r="V9" t="n">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="W9" t="n">
         <v>50</v>
@@ -1908,7 +1908,7 @@
         <v>7.42</v>
       </c>
       <c r="Z9" t="n">
-        <v>-196</v>
+        <v>-55</v>
       </c>
       <c r="AA9" t="n">
         <v>175.89</v>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>'00:06</t>
+          <t>'-00:19</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
@@ -1981,12 +1981,12 @@
       </c>
       <c r="AP9" t="inlineStr">
         <is>
-          <t>'00:04</t>
+          <t>'00:03</t>
         </is>
       </c>
       <c r="AQ9" t="inlineStr">
         <is>
-          <t>'-00:55</t>
+          <t>'-00:51</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
         <v>8.609999999999999</v>
       </c>
       <c r="V10" t="n">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="W10" t="n">
         <v>76</v>
@@ -2069,7 +2069,7 @@
         <v>8.789999999999999</v>
       </c>
       <c r="Z10" t="n">
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="AA10" t="n">
         <v>171.26</v>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>'01:15</t>
+          <t>'-00:06</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">
@@ -2142,12 +2142,12 @@
       </c>
       <c r="AP10" t="inlineStr">
         <is>
-          <t>'00:07</t>
+          <t>'00:05</t>
         </is>
       </c>
       <c r="AQ10" t="inlineStr">
         <is>
-          <t>'-00:04</t>
+          <t>'-00:11</t>
         </is>
       </c>
     </row>
@@ -2218,7 +2218,7 @@
         <v>8.08</v>
       </c>
       <c r="V11" t="n">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="W11" t="n">
         <v>110</v>
@@ -2230,7 +2230,7 @@
         <v>8.609999999999999</v>
       </c>
       <c r="Z11" t="n">
-        <v>260</v>
+        <v>307</v>
       </c>
       <c r="AA11" t="n">
         <v>161.82</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>'01:30</t>
+          <t>'00:39</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
@@ -2303,12 +2303,12 @@
       </c>
       <c r="AP11" t="inlineStr">
         <is>
-          <t>'00:12</t>
+          <t>'00:11</t>
         </is>
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>'-00:04</t>
+          <t>'-00:09</t>
         </is>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
         <v>8.94</v>
       </c>
       <c r="V12" t="n">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="W12" t="n">
         <v>131</v>
@@ -2391,7 +2391,7 @@
         <v>7.7</v>
       </c>
       <c r="Z12" t="n">
-        <v>391</v>
+        <v>541</v>
       </c>
       <c r="AA12" t="n">
         <v>161.53</v>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>'01:45</t>
+          <t>'00:27</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr">
@@ -2464,12 +2464,12 @@
       </c>
       <c r="AP12" t="inlineStr">
         <is>
-          <t>'00:05</t>
+          <t>'00:04</t>
         </is>
       </c>
       <c r="AQ12" t="inlineStr">
         <is>
-          <t>'00:10</t>
+          <t>'00:17</t>
         </is>
       </c>
     </row>
@@ -2540,7 +2540,7 @@
         <v>7.15</v>
       </c>
       <c r="V13" t="n">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="W13" t="n">
         <v>128</v>
@@ -2552,7 +2552,7 @@
         <v>7.78</v>
       </c>
       <c r="Z13" t="n">
-        <v>390</v>
+        <v>521</v>
       </c>
       <c r="AA13" t="n">
         <v>160.37</v>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>'00:26</t>
+          <t>'-00:48</t>
         </is>
       </c>
       <c r="AM13" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="AQ13" t="inlineStr">
         <is>
-          <t>'00:03</t>
+          <t>'00:06</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
         <v>9.640000000000001</v>
       </c>
       <c r="V14" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="W14" t="n">
         <v>61</v>
@@ -2713,7 +2713,7 @@
         <v>6.86</v>
       </c>
       <c r="Z14" t="n">
-        <v>900</v>
+        <v>981</v>
       </c>
       <c r="AA14" t="n">
         <v>160.25</v>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>'00:33</t>
+          <t>'-00:06</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="AQ14" t="inlineStr">
         <is>
-          <t>'01:01</t>
+          <t>'01:00</t>
         </is>
       </c>
     </row>
@@ -2862,7 +2862,7 @@
         <v>7.45</v>
       </c>
       <c r="V15" t="n">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="W15" t="n">
         <v>150</v>
@@ -2874,7 +2874,7 @@
         <v>6.28</v>
       </c>
       <c r="Z15" t="n">
-        <v>782</v>
+        <v>1085</v>
       </c>
       <c r="AA15" t="n">
         <v>160.24</v>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>'00:08</t>
+          <t>'-00:34</t>
         </is>
       </c>
       <c r="AM15" t="inlineStr">
@@ -2947,12 +2947,12 @@
       </c>
       <c r="AP15" t="inlineStr">
         <is>
-          <t>'00:14</t>
+          <t>'00:13</t>
         </is>
       </c>
       <c r="AQ15" t="inlineStr">
         <is>
-          <t>'00:44</t>
+          <t>'01:04</t>
         </is>
       </c>
     </row>
@@ -3023,7 +3023,7 @@
         <v>8.470000000000001</v>
       </c>
       <c r="V16" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="W16" t="n">
         <v>125</v>
@@ -3035,7 +3035,7 @@
         <v>7.79</v>
       </c>
       <c r="Z16" t="n">
-        <v>409</v>
+        <v>523</v>
       </c>
       <c r="AA16" t="n">
         <v>156.49</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>'01:49</t>
+          <t>'-00:14</t>
         </is>
       </c>
       <c r="AM16" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="AQ16" t="inlineStr">
         <is>
-          <t>'00:08</t>
+          <t>'00:10</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
         <v>8.9</v>
       </c>
       <c r="V17" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W17" t="n">
         <v>115</v>
@@ -3196,7 +3196,7 @@
         <v>8.32</v>
       </c>
       <c r="Z17" t="n">
-        <v>313</v>
+        <v>379</v>
       </c>
       <c r="AA17" t="n">
         <v>153.6</v>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>'06:17</t>
+          <t>'02:03</t>
         </is>
       </c>
       <c r="AM17" t="inlineStr">
@@ -3345,7 +3345,7 @@
         <v>7.54</v>
       </c>
       <c r="V18" t="n">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="W18" t="n">
         <v>140</v>
@@ -3357,7 +3357,7 @@
         <v>7.18</v>
       </c>
       <c r="Z18" t="n">
-        <v>494</v>
+        <v>710</v>
       </c>
       <c r="AA18" t="n">
         <v>138.74</v>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>'05:40</t>
+          <t>'01:34</t>
         </is>
       </c>
       <c r="AM18" t="inlineStr">
@@ -3430,12 +3430,12 @@
       </c>
       <c r="AP18" t="inlineStr">
         <is>
-          <t>'00:19</t>
+          <t>'00:16</t>
         </is>
       </c>
       <c r="AQ18" t="inlineStr">
         <is>
-          <t>'00:30</t>
+          <t>'00:48</t>
         </is>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
         <v>9.41</v>
       </c>
       <c r="V19" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W19" t="n">
         <v>92</v>
@@ -3518,7 +3518,7 @@
         <v>8.369999999999999</v>
       </c>
       <c r="Z19" t="n">
-        <v>392</v>
+        <v>407</v>
       </c>
       <c r="AA19" t="n">
         <v>138.12</v>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="AL19" t="inlineStr">
         <is>
-          <t>'04:41</t>
+          <t>'02:54</t>
         </is>
       </c>
       <c r="AM19" t="inlineStr">
@@ -3591,12 +3591,12 @@
       </c>
       <c r="AP19" t="inlineStr">
         <is>
-          <t>'00:02</t>
+          <t>'00:03</t>
         </is>
       </c>
       <c r="AQ19" t="inlineStr">
         <is>
-          <t>'00:24</t>
+          <t>'00:17</t>
         </is>
       </c>
     </row>
@@ -3667,7 +3667,7 @@
         <v>7.44</v>
       </c>
       <c r="V20" t="n">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="W20" t="n">
         <v>104</v>
@@ -3679,7 +3679,7 @@
         <v>8.42</v>
       </c>
       <c r="Z20" t="n">
-        <v>342</v>
+        <v>373</v>
       </c>
       <c r="AA20" t="n">
         <v>134.77</v>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>'10:43</t>
+          <t>'02:51</t>
         </is>
       </c>
       <c r="AM20" t="inlineStr">
@@ -3752,12 +3752,12 @@
       </c>
       <c r="AP20" t="inlineStr">
         <is>
-          <t>'00:23</t>
+          <t>'00:22</t>
         </is>
       </c>
       <c r="AQ20" t="inlineStr">
         <is>
-          <t>'00:16</t>
+          <t>'00:11</t>
         </is>
       </c>
     </row>
@@ -3828,7 +3828,7 @@
         <v>4.82</v>
       </c>
       <c r="V21" t="n">
-        <v>-120</v>
+        <v>-77</v>
       </c>
       <c r="W21" t="n">
         <v>122</v>
@@ -3840,7 +3840,7 @@
         <v>5.83</v>
       </c>
       <c r="Z21" t="n">
-        <v>1305</v>
+        <v>1403</v>
       </c>
       <c r="AA21" t="n">
         <v>132.16</v>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="AL21" t="inlineStr">
         <is>
-          <t>'05:44</t>
+          <t>'02:09</t>
         </is>
       </c>
       <c r="AM21" t="inlineStr">
@@ -3913,12 +3913,12 @@
       </c>
       <c r="AP21" t="inlineStr">
         <is>
-          <t>'-00:20</t>
+          <t>'-00:14</t>
         </is>
       </c>
       <c r="AQ21" t="inlineStr">
         <is>
-          <t>'02:28</t>
+          <t>'02:31</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
         <v>2.47</v>
       </c>
       <c r="V22" t="n">
-        <v>521</v>
+        <v>479</v>
       </c>
       <c r="W22" t="n">
         <v>137</v>
@@ -4001,7 +4001,7 @@
         <v>6.16</v>
       </c>
       <c r="Z22" t="n">
-        <v>990</v>
+        <v>1182</v>
       </c>
       <c r="AA22" t="n">
         <v>118.19</v>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="AL22" t="inlineStr">
         <is>
-          <t>'10:19</t>
+          <t>'01:32</t>
         </is>
       </c>
       <c r="AM22" t="inlineStr">
@@ -4074,12 +4074,12 @@
       </c>
       <c r="AP22" t="inlineStr">
         <is>
-          <t>'01:05</t>
+          <t>'01:00</t>
         </is>
       </c>
       <c r="AQ22" t="inlineStr">
         <is>
-          <t>'01:35</t>
+          <t>'01:50</t>
         </is>
       </c>
     </row>

</xml_diff>